<commit_message>
11/7 updates.. a lot
</commit_message>
<xml_diff>
--- a/homework.xlsx
+++ b/homework.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dccub\OneDrive\바탕 화면\C3Cube-Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dccub\C3Cube-Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465715B8-6C6B-4499-9E8E-C43D10E590D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CC18C7-D6D2-4C45-BE9C-DCCDF1093D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDFF960E-C538-493E-8F04-F63B1A8350B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>CD-P1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -203,6 +203,26 @@
   </si>
   <si>
     <t>자유주제 csv 파일 분석 + 막대/항아리 그래프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>codeup : 6017-6020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>codeup : 4012 (석차계산)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4012(석차계산)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>codeup : 1025-1030</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -650,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DE9F00-5939-4442-9C97-3E67D9434F02}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -703,7 +723,9 @@
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -887,6 +909,9 @@
       <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -912,6 +937,9 @@
       <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="33" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -931,7 +959,13 @@
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -947,6 +981,9 @@
       </c>
       <c r="C28" s="3" t="s">
         <v>36</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>